<commit_message>
yicai spider add some comment beautiful end condition
</commit_message>
<xml_diff>
--- a/thepaper/爬虫列表.xlsx
+++ b/thepaper/爬虫列表.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="259" uniqueCount="159">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="260" uniqueCount="159">
   <si>
     <t>日常新闻转载来源（排名按新闻数量）</t>
   </si>
@@ -447,6 +447,7 @@
         <color rgb="FF0073BF"/>
         <rFont val="Droid Sans Fallback"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">页</t>
     </r>
@@ -458,6 +459,7 @@
         <color rgb="FF0073BF"/>
         <rFont val="Droid Sans Japanese"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">有推荐的文章并不出</t>
     </r>
@@ -469,6 +471,7 @@
         <color rgb="FF0073BF"/>
         <rFont val="Droid Sans Fallback"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">现</t>
     </r>
@@ -480,6 +483,7 @@
         <color rgb="FF0073BF"/>
         <rFont val="Droid Sans Japanese"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">在</t>
     </r>
@@ -491,6 +495,7 @@
         <color rgb="FF0073BF"/>
         <rFont val="DejaVu Sans Mono"/>
         <family val="3"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">api</t>
     </r>
@@ -502,6 +507,7 @@
         <color rgb="FF0073BF"/>
         <rFont val="Droid Sans Japanese"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">中</t>
     </r>
@@ -719,6 +725,7 @@
       <color rgb="FF0073BF"/>
       <name val="Droid Sans Japanese"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <b val="true"/>
@@ -727,6 +734,7 @@
       <color rgb="FF0073BF"/>
       <name val="Droid Sans Fallback"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <b val="true"/>
@@ -735,6 +743,7 @@
       <color rgb="FF0073BF"/>
       <name val="DejaVu Sans Mono"/>
       <family val="3"/>
+      <charset val="1"/>
     </font>
     <font>
       <u val="single"/>
@@ -977,7 +986,7 @@
   <dimension ref="A1:M92"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A10" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D24" activeCellId="1" sqref="E18 D24"/>
+      <selection pane="topLeft" activeCell="D24" activeCellId="1" sqref="E21 D24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -1676,7 +1685,7 @@
   <dimension ref="1:63"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A13" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E18" activeCellId="0" sqref="E18"/>
+      <selection pane="topLeft" activeCell="E21" activeCellId="0" sqref="E21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="11.25"/>
@@ -21283,6 +21292,9 @@
         <v>61</v>
       </c>
       <c r="C21" s="9"/>
+      <c r="E21" s="4" t="s">
+        <v>119</v>
+      </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="7" t="s">
@@ -21306,6 +21318,7 @@
       <c r="C23" s="9" t="s">
         <v>122</v>
       </c>
+      <c r="E23" s="0"/>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="7" t="s">
@@ -21317,6 +21330,7 @@
       <c r="C24" s="9" t="s">
         <v>123</v>
       </c>
+      <c r="E24" s="0"/>
     </row>
     <row r="25" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="7" t="s">
@@ -21328,6 +21342,7 @@
       <c r="C25" s="9" t="s">
         <v>124</v>
       </c>
+      <c r="E25" s="0"/>
     </row>
     <row r="26" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="9" t="s">
@@ -21339,6 +21354,7 @@
       <c r="C26" s="16" t="s">
         <v>127</v>
       </c>
+      <c r="E26" s="0"/>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="7" t="s">
@@ -21362,6 +21378,7 @@
       <c r="C28" s="9" t="s">
         <v>123</v>
       </c>
+      <c r="E28" s="0"/>
     </row>
     <row r="29" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="9" t="s">
@@ -21741,7 +21758,7 @@
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="E18 A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="E21 A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>

</xml_diff>